<commit_message>
Improve disclaimers, add realistic data, and fix desvios críticos
- Remove icon circles from all disclaimers (Despesas, Orçamento, Indicadores, CashFlow)
- Show only filename in 'Arquivo:' field (e.g., Despesas_Exemplo.xlsx)
- Enhance data generation:
  * Use consistent, realistic values per company
  * Add seed(42) for reproducible test data
  * Cash Flow: 1046 registros com valores distribuídos
  * Indicadores: 36 registros com métricas financeiras realistas
  * Orçamento: 360 registros com desvios variados (75-135%)
  * Despesas: 3600 registros distribuídos por 8 categorias
- Fix 'Desvios Críticos' table in Orçamento:
  * Filter desvios by selected empresa
  * Calculate from filtered data, not global data
  * Remove unused obterDesviosPorCategoria from dependency
- All Excel files regenerated with improved test data
</commit_message>
<xml_diff>
--- a/dados/excel_exemplos/Indicadores_Exemplo.xlsx
+++ b/dados/excel_exemplos/Indicadores_Exemplo.xlsx
@@ -526,37 +526,37 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>37.9</v>
+        <v>14.91</v>
       </c>
       <c r="D2" t="n">
-        <v>13.35</v>
+        <v>9.710000000000001</v>
       </c>
       <c r="E2" t="n">
-        <v>17.15</v>
+        <v>17.36</v>
       </c>
       <c r="F2" t="n">
-        <v>34.55</v>
+        <v>18.87</v>
       </c>
       <c r="G2" t="n">
-        <v>3.07</v>
+        <v>1.92</v>
       </c>
       <c r="H2" t="n">
-        <v>1.95</v>
+        <v>1.15</v>
       </c>
       <c r="I2" t="n">
-        <v>52.63</v>
+        <v>48.03</v>
       </c>
       <c r="J2" t="n">
-        <v>2.81</v>
+        <v>2.4</v>
       </c>
       <c r="K2" t="n">
-        <v>1.06</v>
+        <v>2.49</v>
       </c>
       <c r="L2" t="n">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M2" t="n">
-        <v>74</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3">
@@ -569,37 +569,37 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>12.5</v>
+        <v>18.81</v>
       </c>
       <c r="D3" t="n">
-        <v>19.05</v>
+        <v>10.55</v>
       </c>
       <c r="E3" t="n">
-        <v>23.25</v>
+        <v>13.83</v>
       </c>
       <c r="F3" t="n">
-        <v>10.3</v>
+        <v>23.66</v>
       </c>
       <c r="G3" t="n">
-        <v>2.43</v>
+        <v>2.7</v>
       </c>
       <c r="H3" t="n">
-        <v>1.4</v>
+        <v>1.46</v>
       </c>
       <c r="I3" t="n">
-        <v>53.45</v>
+        <v>41.48</v>
       </c>
       <c r="J3" t="n">
-        <v>3.07</v>
+        <v>2.72</v>
       </c>
       <c r="K3" t="n">
-        <v>3.81</v>
+        <v>2.49</v>
       </c>
       <c r="L3" t="n">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="M3" t="n">
-        <v>22</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4">
@@ -612,37 +612,37 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>13.85</v>
+        <v>17.08</v>
       </c>
       <c r="D4" t="n">
-        <v>16.95</v>
+        <v>10.32</v>
       </c>
       <c r="E4" t="n">
-        <v>24.44</v>
+        <v>15.53</v>
       </c>
       <c r="F4" t="n">
-        <v>32.2</v>
+        <v>21.47</v>
       </c>
       <c r="G4" t="n">
-        <v>3.15</v>
+        <v>2.4</v>
       </c>
       <c r="H4" t="n">
-        <v>2.08</v>
+        <v>1.9</v>
       </c>
       <c r="I4" t="n">
-        <v>37.4</v>
+        <v>46.09</v>
       </c>
       <c r="J4" t="n">
-        <v>3.48</v>
+        <v>2.2</v>
       </c>
       <c r="K4" t="n">
-        <v>3.73</v>
+        <v>1.51</v>
       </c>
       <c r="L4" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M4" t="n">
-        <v>66</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5">
@@ -655,37 +655,37 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>23.34</v>
+        <v>16.9</v>
       </c>
       <c r="D5" t="n">
-        <v>14.96</v>
+        <v>9.9</v>
       </c>
       <c r="E5" t="n">
-        <v>7.9</v>
+        <v>13.8</v>
       </c>
       <c r="F5" t="n">
-        <v>34.93</v>
+        <v>18.66</v>
       </c>
       <c r="G5" t="n">
-        <v>2.74</v>
+        <v>2.68</v>
       </c>
       <c r="H5" t="n">
-        <v>0.98</v>
+        <v>1.43</v>
       </c>
       <c r="I5" t="n">
-        <v>41.5</v>
+        <v>50.48</v>
       </c>
       <c r="J5" t="n">
-        <v>1.46</v>
+        <v>3.12</v>
       </c>
       <c r="K5" t="n">
-        <v>2.56</v>
+        <v>1.78</v>
       </c>
       <c r="L5" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="M5" t="n">
-        <v>66</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
@@ -698,37 +698,37 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>25.12</v>
+        <v>20.68</v>
       </c>
       <c r="D6" t="n">
-        <v>14.02</v>
+        <v>10.21</v>
       </c>
       <c r="E6" t="n">
-        <v>6.65</v>
+        <v>18.59</v>
       </c>
       <c r="F6" t="n">
-        <v>15.77</v>
+        <v>20.53</v>
       </c>
       <c r="G6" t="n">
-        <v>1.83</v>
+        <v>1.77</v>
       </c>
       <c r="H6" t="n">
-        <v>1.85</v>
+        <v>1.27</v>
       </c>
       <c r="I6" t="n">
-        <v>68.29000000000001</v>
+        <v>47.41</v>
       </c>
       <c r="J6" t="n">
-        <v>3.54</v>
+        <v>2</v>
       </c>
       <c r="K6" t="n">
-        <v>3.13</v>
+        <v>2.89</v>
       </c>
       <c r="L6" t="n">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="M6" t="n">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7">
@@ -741,37 +741,37 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>30.08</v>
+        <v>19.86</v>
       </c>
       <c r="D7" t="n">
-        <v>14.11</v>
+        <v>10.78</v>
       </c>
       <c r="E7" t="n">
-        <v>16.26</v>
+        <v>15.55</v>
       </c>
       <c r="F7" t="n">
-        <v>14.28</v>
+        <v>18.32</v>
       </c>
       <c r="G7" t="n">
-        <v>2.69</v>
+        <v>1.64</v>
       </c>
       <c r="H7" t="n">
-        <v>0.89</v>
+        <v>1.7</v>
       </c>
       <c r="I7" t="n">
-        <v>33.19</v>
+        <v>39.3</v>
       </c>
       <c r="J7" t="n">
-        <v>4.33</v>
+        <v>2.81</v>
       </c>
       <c r="K7" t="n">
-        <v>3.1</v>
+        <v>1.82</v>
       </c>
       <c r="L7" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M7" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8">
@@ -784,37 +784,37 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>35.11</v>
+        <v>15.13</v>
       </c>
       <c r="D8" t="n">
-        <v>16.88</v>
+        <v>8.98</v>
       </c>
       <c r="E8" t="n">
-        <v>16.43</v>
+        <v>13.07</v>
       </c>
       <c r="F8" t="n">
-        <v>31.39</v>
+        <v>22.99</v>
       </c>
       <c r="G8" t="n">
-        <v>3.14</v>
+        <v>2.04</v>
       </c>
       <c r="H8" t="n">
-        <v>1.62</v>
+        <v>1.92</v>
       </c>
       <c r="I8" t="n">
-        <v>22.03</v>
+        <v>39.09</v>
       </c>
       <c r="J8" t="n">
-        <v>3.52</v>
+        <v>2.04</v>
       </c>
       <c r="K8" t="n">
-        <v>2.96</v>
+        <v>2.55</v>
       </c>
       <c r="L8" t="n">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="M8" t="n">
-        <v>23</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9">
@@ -827,37 +827,37 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>29.78</v>
+        <v>17.29</v>
       </c>
       <c r="D9" t="n">
-        <v>12.7</v>
+        <v>9.35</v>
       </c>
       <c r="E9" t="n">
-        <v>19.65</v>
+        <v>17.69</v>
       </c>
       <c r="F9" t="n">
-        <v>23.03</v>
+        <v>22.17</v>
       </c>
       <c r="G9" t="n">
-        <v>2.4</v>
+        <v>1.87</v>
       </c>
       <c r="H9" t="n">
-        <v>1.02</v>
+        <v>1.19</v>
       </c>
       <c r="I9" t="n">
-        <v>50.51</v>
+        <v>51.43</v>
       </c>
       <c r="J9" t="n">
-        <v>1.44</v>
+        <v>1.85</v>
       </c>
       <c r="K9" t="n">
-        <v>3.14</v>
+        <v>3</v>
       </c>
       <c r="L9" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="M9" t="n">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10">
@@ -870,37 +870,37 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>31.5</v>
+        <v>14.09</v>
       </c>
       <c r="D10" t="n">
-        <v>14.12</v>
+        <v>11.33</v>
       </c>
       <c r="E10" t="n">
-        <v>14.61</v>
+        <v>17.08</v>
       </c>
       <c r="F10" t="n">
-        <v>31.5</v>
+        <v>23.26</v>
       </c>
       <c r="G10" t="n">
-        <v>3.12</v>
+        <v>2.22</v>
       </c>
       <c r="H10" t="n">
-        <v>1.93</v>
+        <v>2</v>
       </c>
       <c r="I10" t="n">
-        <v>16.71</v>
+        <v>52.57</v>
       </c>
       <c r="J10" t="n">
-        <v>3.76</v>
+        <v>2.65</v>
       </c>
       <c r="K10" t="n">
-        <v>3.76</v>
+        <v>2.92</v>
       </c>
       <c r="L10" t="n">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="M10" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11">
@@ -913,37 +913,37 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>15.11</v>
+        <v>16.17</v>
       </c>
       <c r="D11" t="n">
-        <v>8.16</v>
+        <v>8.369999999999999</v>
       </c>
       <c r="E11" t="n">
-        <v>21.81</v>
+        <v>15.27</v>
       </c>
       <c r="F11" t="n">
-        <v>13.23</v>
+        <v>23.71</v>
       </c>
       <c r="G11" t="n">
-        <v>1.88</v>
+        <v>2.47</v>
       </c>
       <c r="H11" t="n">
-        <v>1.16</v>
+        <v>1.48</v>
       </c>
       <c r="I11" t="n">
-        <v>62.58</v>
+        <v>26.68</v>
       </c>
       <c r="J11" t="n">
-        <v>4.08</v>
+        <v>2.47</v>
       </c>
       <c r="K11" t="n">
-        <v>3.41</v>
+        <v>3.15</v>
       </c>
       <c r="L11" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="M11" t="n">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12">
@@ -956,37 +956,37 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>10.78</v>
+        <v>20.53</v>
       </c>
       <c r="D12" t="n">
-        <v>12.06</v>
+        <v>9.869999999999999</v>
       </c>
       <c r="E12" t="n">
-        <v>5.64</v>
+        <v>14.88</v>
       </c>
       <c r="F12" t="n">
-        <v>18.56</v>
+        <v>21.85</v>
       </c>
       <c r="G12" t="n">
-        <v>2.4</v>
+        <v>2.58</v>
       </c>
       <c r="H12" t="n">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="I12" t="n">
-        <v>32.32</v>
+        <v>49.1</v>
       </c>
       <c r="J12" t="n">
-        <v>1.79</v>
+        <v>2.9</v>
       </c>
       <c r="K12" t="n">
-        <v>1.4</v>
+        <v>1.89</v>
       </c>
       <c r="L12" t="n">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="M12" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13">
@@ -999,37 +999,37 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>8.19</v>
+        <v>14.62</v>
       </c>
       <c r="D13" t="n">
-        <v>15.72</v>
+        <v>10.41</v>
       </c>
       <c r="E13" t="n">
-        <v>23.59</v>
+        <v>18.08</v>
       </c>
       <c r="F13" t="n">
-        <v>25.84</v>
+        <v>18.17</v>
       </c>
       <c r="G13" t="n">
-        <v>1.84</v>
+        <v>1.87</v>
       </c>
       <c r="H13" t="n">
-        <v>1.76</v>
+        <v>1.65</v>
       </c>
       <c r="I13" t="n">
-        <v>37.8</v>
+        <v>26.96</v>
       </c>
       <c r="J13" t="n">
-        <v>3.19</v>
+        <v>2.82</v>
       </c>
       <c r="K13" t="n">
-        <v>0.89</v>
+        <v>3.01</v>
       </c>
       <c r="L13" t="n">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="M13" t="n">
-        <v>72</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14">
@@ -1042,37 +1042,37 @@
         </is>
       </c>
       <c r="C14" t="n">
+        <v>22.41</v>
+      </c>
+      <c r="D14" t="n">
+        <v>12.55</v>
+      </c>
+      <c r="E14" t="n">
+        <v>15.19</v>
+      </c>
+      <c r="F14" t="n">
         <v>21.62</v>
       </c>
-      <c r="D14" t="n">
-        <v>8.539999999999999</v>
-      </c>
-      <c r="E14" t="n">
-        <v>9.1</v>
-      </c>
-      <c r="F14" t="n">
-        <v>30.84</v>
-      </c>
       <c r="G14" t="n">
-        <v>2.74</v>
+        <v>2.77</v>
       </c>
       <c r="H14" t="n">
-        <v>0.82</v>
+        <v>1.68</v>
       </c>
       <c r="I14" t="n">
-        <v>36.41</v>
+        <v>41.91</v>
       </c>
       <c r="J14" t="n">
-        <v>2.14</v>
+        <v>3.14</v>
       </c>
       <c r="K14" t="n">
-        <v>1.87</v>
+        <v>1.59</v>
       </c>
       <c r="L14" t="n">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="M14" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15">
@@ -1085,37 +1085,37 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>13.48</v>
+        <v>25.55</v>
       </c>
       <c r="D15" t="n">
-        <v>3.37</v>
+        <v>10.03</v>
       </c>
       <c r="E15" t="n">
-        <v>14.26</v>
+        <v>17.14</v>
       </c>
       <c r="F15" t="n">
-        <v>23.11</v>
+        <v>21.69</v>
       </c>
       <c r="G15" t="n">
-        <v>1.46</v>
+        <v>2.02</v>
       </c>
       <c r="H15" t="n">
-        <v>2.3</v>
+        <v>1.23</v>
       </c>
       <c r="I15" t="n">
-        <v>50.01</v>
+        <v>47.56</v>
       </c>
       <c r="J15" t="n">
-        <v>1.38</v>
+        <v>3.03</v>
       </c>
       <c r="K15" t="n">
-        <v>2.29</v>
+        <v>3.45</v>
       </c>
       <c r="L15" t="n">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="M15" t="n">
-        <v>64</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16">
@@ -1128,37 +1128,37 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>30.71</v>
+        <v>20.65</v>
       </c>
       <c r="D16" t="n">
-        <v>5.6</v>
+        <v>13.59</v>
       </c>
       <c r="E16" t="n">
-        <v>14.69</v>
+        <v>18.02</v>
       </c>
       <c r="F16" t="n">
-        <v>12.04</v>
+        <v>23.01</v>
       </c>
       <c r="G16" t="n">
-        <v>1.99</v>
+        <v>2.51</v>
       </c>
       <c r="H16" t="n">
-        <v>1.54</v>
+        <v>1.03</v>
       </c>
       <c r="I16" t="n">
-        <v>55.59</v>
+        <v>48.88</v>
       </c>
       <c r="J16" t="n">
-        <v>3.42</v>
+        <v>2.61</v>
       </c>
       <c r="K16" t="n">
-        <v>2.12</v>
+        <v>3.24</v>
       </c>
       <c r="L16" t="n">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="M16" t="n">
-        <v>65</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17">
@@ -1171,37 +1171,37 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>23.25</v>
+        <v>19.29</v>
       </c>
       <c r="D17" t="n">
-        <v>5.64</v>
+        <v>12.73</v>
       </c>
       <c r="E17" t="n">
-        <v>23.49</v>
+        <v>15.47</v>
       </c>
       <c r="F17" t="n">
-        <v>17.24</v>
+        <v>23.76</v>
       </c>
       <c r="G17" t="n">
-        <v>1.99</v>
+        <v>2.74</v>
       </c>
       <c r="H17" t="n">
-        <v>1.1</v>
+        <v>1.28</v>
       </c>
       <c r="I17" t="n">
-        <v>41.08</v>
+        <v>31.47</v>
       </c>
       <c r="J17" t="n">
-        <v>3.46</v>
+        <v>2.96</v>
       </c>
       <c r="K17" t="n">
-        <v>2.54</v>
+        <v>1.78</v>
       </c>
       <c r="L17" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="M17" t="n">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18">
@@ -1214,37 +1214,37 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>20.57</v>
+        <v>25.95</v>
       </c>
       <c r="D18" t="n">
-        <v>12.93</v>
+        <v>12.01</v>
       </c>
       <c r="E18" t="n">
-        <v>23.22</v>
+        <v>20.95</v>
       </c>
       <c r="F18" t="n">
-        <v>15.34</v>
+        <v>23.65</v>
       </c>
       <c r="G18" t="n">
-        <v>1.76</v>
+        <v>2.18</v>
       </c>
       <c r="H18" t="n">
-        <v>1.41</v>
+        <v>1.92</v>
       </c>
       <c r="I18" t="n">
-        <v>69.18000000000001</v>
+        <v>38.42</v>
       </c>
       <c r="J18" t="n">
-        <v>3.01</v>
+        <v>2.02</v>
       </c>
       <c r="K18" t="n">
-        <v>1.07</v>
+        <v>2.08</v>
       </c>
       <c r="L18" t="n">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="M18" t="n">
-        <v>30</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19">
@@ -1257,37 +1257,37 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>22.75</v>
+        <v>18.32</v>
       </c>
       <c r="D19" t="n">
-        <v>16.97</v>
+        <v>12.85</v>
       </c>
       <c r="E19" t="n">
-        <v>13.13</v>
+        <v>19.1</v>
       </c>
       <c r="F19" t="n">
-        <v>15.78</v>
+        <v>21.43</v>
       </c>
       <c r="G19" t="n">
-        <v>1.97</v>
+        <v>2.8</v>
       </c>
       <c r="H19" t="n">
-        <v>1.9</v>
+        <v>1.73</v>
       </c>
       <c r="I19" t="n">
-        <v>52.51</v>
+        <v>53.74</v>
       </c>
       <c r="J19" t="n">
-        <v>1.43</v>
+        <v>2.76</v>
       </c>
       <c r="K19" t="n">
-        <v>3.01</v>
+        <v>3.49</v>
       </c>
       <c r="L19" t="n">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="M19" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20">
@@ -1300,37 +1300,37 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>10.38</v>
+        <v>19.14</v>
       </c>
       <c r="D20" t="n">
-        <v>16.24</v>
+        <v>13.48</v>
       </c>
       <c r="E20" t="n">
-        <v>13.71</v>
+        <v>18.28</v>
       </c>
       <c r="F20" t="n">
-        <v>26.27</v>
+        <v>25.81</v>
       </c>
       <c r="G20" t="n">
-        <v>1.98</v>
+        <v>2.52</v>
       </c>
       <c r="H20" t="n">
-        <v>0.93</v>
+        <v>1.1</v>
       </c>
       <c r="I20" t="n">
-        <v>15.13</v>
+        <v>27.82</v>
       </c>
       <c r="J20" t="n">
-        <v>4.15</v>
+        <v>2.33</v>
       </c>
       <c r="K20" t="n">
-        <v>2.49</v>
+        <v>3.37</v>
       </c>
       <c r="L20" t="n">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="M20" t="n">
-        <v>55</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21">
@@ -1343,37 +1343,37 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>11.41</v>
+        <v>20.24</v>
       </c>
       <c r="D21" t="n">
-        <v>15.55</v>
+        <v>11.45</v>
       </c>
       <c r="E21" t="n">
-        <v>23.88</v>
+        <v>15.54</v>
       </c>
       <c r="F21" t="n">
-        <v>18.67</v>
+        <v>21.08</v>
       </c>
       <c r="G21" t="n">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="H21" t="n">
-        <v>0.8</v>
+        <v>1.31</v>
       </c>
       <c r="I21" t="n">
-        <v>61.05</v>
+        <v>39.2</v>
       </c>
       <c r="J21" t="n">
-        <v>2.42</v>
+        <v>2.24</v>
       </c>
       <c r="K21" t="n">
-        <v>1.41</v>
+        <v>3.25</v>
       </c>
       <c r="L21" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M21" t="n">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22">
@@ -1386,34 +1386,34 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>33.51</v>
+        <v>25.52</v>
       </c>
       <c r="D22" t="n">
-        <v>9.130000000000001</v>
+        <v>13.89</v>
       </c>
       <c r="E22" t="n">
-        <v>18.73</v>
+        <v>17.93</v>
       </c>
       <c r="F22" t="n">
-        <v>17.69</v>
+        <v>22.18</v>
       </c>
       <c r="G22" t="n">
-        <v>2.7</v>
+        <v>1.87</v>
       </c>
       <c r="H22" t="n">
-        <v>1.35</v>
+        <v>1.49</v>
       </c>
       <c r="I22" t="n">
-        <v>69.19</v>
+        <v>43.59</v>
       </c>
       <c r="J22" t="n">
-        <v>1.82</v>
+        <v>2.96</v>
       </c>
       <c r="K22" t="n">
-        <v>3.43</v>
+        <v>2.38</v>
       </c>
       <c r="L22" t="n">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="M22" t="n">
         <v>45</v>
@@ -1429,37 +1429,37 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>22.7</v>
+        <v>20.99</v>
       </c>
       <c r="D23" t="n">
-        <v>15.76</v>
+        <v>12.73</v>
       </c>
       <c r="E23" t="n">
-        <v>15.4</v>
+        <v>18.04</v>
       </c>
       <c r="F23" t="n">
-        <v>33.68</v>
+        <v>21.58</v>
       </c>
       <c r="G23" t="n">
-        <v>3.15</v>
+        <v>2.64</v>
       </c>
       <c r="H23" t="n">
-        <v>2.17</v>
+        <v>1.82</v>
       </c>
       <c r="I23" t="n">
-        <v>28.39</v>
+        <v>43.62</v>
       </c>
       <c r="J23" t="n">
-        <v>3.4</v>
+        <v>2.89</v>
       </c>
       <c r="K23" t="n">
-        <v>1.72</v>
+        <v>2.98</v>
       </c>
       <c r="L23" t="n">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="M23" t="n">
-        <v>22</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24">
@@ -1472,37 +1472,37 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>16.82</v>
+        <v>18.06</v>
       </c>
       <c r="D24" t="n">
-        <v>9.210000000000001</v>
+        <v>13.41</v>
       </c>
       <c r="E24" t="n">
-        <v>11.3</v>
+        <v>16.74</v>
       </c>
       <c r="F24" t="n">
-        <v>34.06</v>
+        <v>20.95</v>
       </c>
       <c r="G24" t="n">
-        <v>3.3</v>
+        <v>2.02</v>
       </c>
       <c r="H24" t="n">
-        <v>2.4</v>
+        <v>1.09</v>
       </c>
       <c r="I24" t="n">
-        <v>55.83</v>
+        <v>36.65</v>
       </c>
       <c r="J24" t="n">
-        <v>2.53</v>
+        <v>2.59</v>
       </c>
       <c r="K24" t="n">
-        <v>2.95</v>
+        <v>1.69</v>
       </c>
       <c r="L24" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="M24" t="n">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25">
@@ -1515,37 +1515,37 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>25.85</v>
+        <v>23.14</v>
       </c>
       <c r="D25" t="n">
-        <v>4.4</v>
+        <v>13.6</v>
       </c>
       <c r="E25" t="n">
-        <v>12.46</v>
+        <v>17.79</v>
       </c>
       <c r="F25" t="n">
-        <v>32.09</v>
+        <v>20.51</v>
       </c>
       <c r="G25" t="n">
-        <v>3.42</v>
+        <v>2.45</v>
       </c>
       <c r="H25" t="n">
-        <v>2.06</v>
+        <v>2.1</v>
       </c>
       <c r="I25" t="n">
-        <v>42.45</v>
+        <v>52.67</v>
       </c>
       <c r="J25" t="n">
-        <v>2.12</v>
+        <v>3.11</v>
       </c>
       <c r="K25" t="n">
-        <v>2.81</v>
+        <v>1.9</v>
       </c>
       <c r="L25" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M25" t="n">
-        <v>59</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26">
@@ -1558,37 +1558,37 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>24.76</v>
+        <v>13.54</v>
       </c>
       <c r="D26" t="n">
-        <v>21.01</v>
+        <v>9.99</v>
       </c>
       <c r="E26" t="n">
-        <v>18.17</v>
+        <v>11.92</v>
       </c>
       <c r="F26" t="n">
-        <v>32.46</v>
+        <v>18.21</v>
       </c>
       <c r="G26" t="n">
-        <v>2.95</v>
+        <v>2.12</v>
       </c>
       <c r="H26" t="n">
-        <v>1.63</v>
+        <v>1.33</v>
       </c>
       <c r="I26" t="n">
-        <v>43.48</v>
+        <v>26.15</v>
       </c>
       <c r="J26" t="n">
-        <v>4.32</v>
+        <v>2.06</v>
       </c>
       <c r="K26" t="n">
-        <v>3.13</v>
+        <v>2.44</v>
       </c>
       <c r="L26" t="n">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="M26" t="n">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27">
@@ -1601,37 +1601,37 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>19.01</v>
+        <v>13.56</v>
       </c>
       <c r="D27" t="n">
-        <v>9.59</v>
+        <v>6.13</v>
       </c>
       <c r="E27" t="n">
-        <v>5.5</v>
+        <v>12.61</v>
       </c>
       <c r="F27" t="n">
-        <v>19.87</v>
+        <v>16.28</v>
       </c>
       <c r="G27" t="n">
-        <v>1.82</v>
+        <v>2.72</v>
       </c>
       <c r="H27" t="n">
-        <v>1.25</v>
+        <v>1.43</v>
       </c>
       <c r="I27" t="n">
-        <v>61.58</v>
+        <v>37.9</v>
       </c>
       <c r="J27" t="n">
-        <v>2.25</v>
+        <v>2.6</v>
       </c>
       <c r="K27" t="n">
-        <v>3.59</v>
+        <v>1.61</v>
       </c>
       <c r="L27" t="n">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="M27" t="n">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28">
@@ -1644,37 +1644,37 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>30.55</v>
+        <v>18.62</v>
       </c>
       <c r="D28" t="n">
-        <v>18.54</v>
+        <v>8.73</v>
       </c>
       <c r="E28" t="n">
-        <v>12.93</v>
+        <v>10.62</v>
       </c>
       <c r="F28" t="n">
-        <v>26.81</v>
+        <v>17.81</v>
       </c>
       <c r="G28" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="I28" t="n">
+        <v>37.15</v>
+      </c>
+      <c r="J28" t="n">
         <v>2.31</v>
       </c>
-      <c r="H28" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="I28" t="n">
-        <v>33.04</v>
-      </c>
-      <c r="J28" t="n">
-        <v>3.23</v>
-      </c>
       <c r="K28" t="n">
-        <v>3.05</v>
+        <v>2.92</v>
       </c>
       <c r="L28" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M28" t="n">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29">
@@ -1687,37 +1687,37 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>26.12</v>
+        <v>15.2</v>
       </c>
       <c r="D29" t="n">
-        <v>7.08</v>
+        <v>8.68</v>
       </c>
       <c r="E29" t="n">
-        <v>18.07</v>
+        <v>10.56</v>
       </c>
       <c r="F29" t="n">
-        <v>10.19</v>
+        <v>18.98</v>
       </c>
       <c r="G29" t="n">
-        <v>2.09</v>
+        <v>1.62</v>
       </c>
       <c r="H29" t="n">
-        <v>1.59</v>
+        <v>2.08</v>
       </c>
       <c r="I29" t="n">
-        <v>29.87</v>
+        <v>35.26</v>
       </c>
       <c r="J29" t="n">
-        <v>2.86</v>
+        <v>3.08</v>
       </c>
       <c r="K29" t="n">
-        <v>1.44</v>
+        <v>1.83</v>
       </c>
       <c r="L29" t="n">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="M29" t="n">
-        <v>37</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30">
@@ -1730,37 +1730,37 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>13.79</v>
+        <v>14.85</v>
       </c>
       <c r="D30" t="n">
-        <v>12.49</v>
+        <v>8.140000000000001</v>
       </c>
       <c r="E30" t="n">
-        <v>19.28</v>
+        <v>13.7</v>
       </c>
       <c r="F30" t="n">
-        <v>27.38</v>
+        <v>19.79</v>
       </c>
       <c r="G30" t="n">
-        <v>3.03</v>
+        <v>2.07</v>
       </c>
       <c r="H30" t="n">
-        <v>1.41</v>
+        <v>2.1</v>
       </c>
       <c r="I30" t="n">
-        <v>48.08</v>
+        <v>42.11</v>
       </c>
       <c r="J30" t="n">
-        <v>3.52</v>
+        <v>3.2</v>
       </c>
       <c r="K30" t="n">
-        <v>0.98</v>
+        <v>2.62</v>
       </c>
       <c r="L30" t="n">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="M30" t="n">
-        <v>73</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31">
@@ -1773,37 +1773,37 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>12.04</v>
+        <v>11.62</v>
       </c>
       <c r="D31" t="n">
-        <v>6.21</v>
+        <v>8.67</v>
       </c>
       <c r="E31" t="n">
-        <v>23.39</v>
+        <v>12.7</v>
       </c>
       <c r="F31" t="n">
-        <v>25</v>
+        <v>15.94</v>
       </c>
       <c r="G31" t="n">
-        <v>2.89</v>
+        <v>2.78</v>
       </c>
       <c r="H31" t="n">
-        <v>2.42</v>
+        <v>2.13</v>
       </c>
       <c r="I31" t="n">
-        <v>28.15</v>
+        <v>47.29</v>
       </c>
       <c r="J31" t="n">
-        <v>3.4</v>
+        <v>3.05</v>
       </c>
       <c r="K31" t="n">
-        <v>3.98</v>
+        <v>2.13</v>
       </c>
       <c r="L31" t="n">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="M31" t="n">
-        <v>33</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32">
@@ -1816,37 +1816,37 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>6.26</v>
+        <v>18.47</v>
       </c>
       <c r="D32" t="n">
-        <v>5.11</v>
+        <v>8</v>
       </c>
       <c r="E32" t="n">
-        <v>15.59</v>
+        <v>10.9</v>
       </c>
       <c r="F32" t="n">
-        <v>17.09</v>
+        <v>18.75</v>
       </c>
       <c r="G32" t="n">
-        <v>1.54</v>
+        <v>2.38</v>
       </c>
       <c r="H32" t="n">
-        <v>2.07</v>
+        <v>1.32</v>
       </c>
       <c r="I32" t="n">
-        <v>64.3</v>
+        <v>46.67</v>
       </c>
       <c r="J32" t="n">
-        <v>2.39</v>
+        <v>3.48</v>
       </c>
       <c r="K32" t="n">
-        <v>2.24</v>
+        <v>3.39</v>
       </c>
       <c r="L32" t="n">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="M32" t="n">
-        <v>58</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33">
@@ -1859,37 +1859,37 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>19.93</v>
+        <v>16.07</v>
       </c>
       <c r="D33" t="n">
-        <v>12.22</v>
+        <v>8.56</v>
       </c>
       <c r="E33" t="n">
-        <v>12.15</v>
+        <v>12.47</v>
       </c>
       <c r="F33" t="n">
-        <v>31.55</v>
+        <v>14.22</v>
       </c>
       <c r="G33" t="n">
-        <v>2.33</v>
+        <v>2.47</v>
       </c>
       <c r="H33" t="n">
-        <v>1.3</v>
+        <v>1.23</v>
       </c>
       <c r="I33" t="n">
-        <v>31.51</v>
+        <v>45.89</v>
       </c>
       <c r="J33" t="n">
-        <v>2.3</v>
+        <v>3.12</v>
       </c>
       <c r="K33" t="n">
-        <v>3.77</v>
+        <v>2.7</v>
       </c>
       <c r="L33" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="M33" t="n">
-        <v>75</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34">
@@ -1902,37 +1902,37 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>24.47</v>
+        <v>12.68</v>
       </c>
       <c r="D34" t="n">
-        <v>16.86</v>
+        <v>6.76</v>
       </c>
       <c r="E34" t="n">
-        <v>8.949999999999999</v>
+        <v>13.08</v>
       </c>
       <c r="F34" t="n">
-        <v>29.35</v>
+        <v>19.73</v>
       </c>
       <c r="G34" t="n">
-        <v>3.2</v>
+        <v>1.98</v>
       </c>
       <c r="H34" t="n">
-        <v>0.91</v>
+        <v>1.44</v>
       </c>
       <c r="I34" t="n">
-        <v>47.01</v>
+        <v>34.06</v>
       </c>
       <c r="J34" t="n">
-        <v>3</v>
+        <v>2.32</v>
       </c>
       <c r="K34" t="n">
-        <v>2.51</v>
+        <v>3.14</v>
       </c>
       <c r="L34" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M34" t="n">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35">
@@ -1945,37 +1945,37 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>10.73</v>
+        <v>16.19</v>
       </c>
       <c r="D35" t="n">
-        <v>7.08</v>
+        <v>7.82</v>
       </c>
       <c r="E35" t="n">
-        <v>21.38</v>
+        <v>11.46</v>
       </c>
       <c r="F35" t="n">
-        <v>14.38</v>
+        <v>16.11</v>
       </c>
       <c r="G35" t="n">
-        <v>3.37</v>
+        <v>2.21</v>
       </c>
       <c r="H35" t="n">
-        <v>1.18</v>
+        <v>1.63</v>
       </c>
       <c r="I35" t="n">
-        <v>64.29000000000001</v>
+        <v>47.95</v>
       </c>
       <c r="J35" t="n">
-        <v>4.49</v>
+        <v>1.99</v>
       </c>
       <c r="K35" t="n">
-        <v>2.81</v>
+        <v>1.85</v>
       </c>
       <c r="L35" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M35" t="n">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36">
@@ -1988,37 +1988,37 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>18.48</v>
+        <v>12.42</v>
       </c>
       <c r="D36" t="n">
-        <v>17.2</v>
+        <v>8.380000000000001</v>
       </c>
       <c r="E36" t="n">
-        <v>5.8</v>
+        <v>12.26</v>
       </c>
       <c r="F36" t="n">
-        <v>28.12</v>
+        <v>16.29</v>
       </c>
       <c r="G36" t="n">
-        <v>3.13</v>
+        <v>2.6</v>
       </c>
       <c r="H36" t="n">
-        <v>1.79</v>
+        <v>1.83</v>
       </c>
       <c r="I36" t="n">
-        <v>35.14</v>
+        <v>38.12</v>
       </c>
       <c r="J36" t="n">
-        <v>3.67</v>
+        <v>2.28</v>
       </c>
       <c r="K36" t="n">
-        <v>3.3</v>
+        <v>2.74</v>
       </c>
       <c r="L36" t="n">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="M36" t="n">
-        <v>49</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37">
@@ -2031,37 +2031,37 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>20.48</v>
+        <v>18.96</v>
       </c>
       <c r="D37" t="n">
-        <v>6.91</v>
+        <v>9.220000000000001</v>
       </c>
       <c r="E37" t="n">
-        <v>10.34</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="F37" t="n">
-        <v>32.95</v>
+        <v>17.9</v>
       </c>
       <c r="G37" t="n">
-        <v>1.5</v>
+        <v>2.3</v>
       </c>
       <c r="H37" t="n">
-        <v>0.88</v>
+        <v>1.49</v>
       </c>
       <c r="I37" t="n">
-        <v>47.43</v>
+        <v>39.89</v>
       </c>
       <c r="J37" t="n">
-        <v>1.24</v>
+        <v>3.08</v>
       </c>
       <c r="K37" t="n">
-        <v>1.29</v>
+        <v>3.35</v>
       </c>
       <c r="L37" t="n">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="M37" t="n">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>